<commit_message>
added save process functionality
on every main functions
</commit_message>
<xml_diff>
--- a/demo_scripts/Feeding_demo_data/metadata.xlsx
+++ b/demo_scripts/Feeding_demo_data/metadata.xlsx
@@ -24,67 +24,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Experiment</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>DEMO waterMED with 48h WD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Folder</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>Group</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>Start</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEMO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>MouseID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Folder</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Start</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>End</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEMO waterMED with 48h WD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EMO</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EMO</t>
-    </r>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -458,7 +428,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -471,24 +441,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -499,7 +469,13 @@
         <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>70522</v>
+      </c>
+      <c r="E3" s="1">
+        <v>286126</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -510,7 +486,13 @@
         <v>380</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>107666</v>
+      </c>
+      <c r="E4" s="1">
+        <v>289620</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>